<commit_message>
Analysis debugging, need to check database and df
</commit_message>
<xml_diff>
--- a/Results_ZC/results_Demand_5.xlsx
+++ b/Results_ZC/results_Demand_5.xlsx
@@ -1,13 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FTNC_Demand5" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="FTNC_Demand5" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="FTNC_Demand51" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="FTNC_Demand52" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="FTNC_Demand53" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="FTNC_Demand54" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="FTNC_Demand55" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -53,18 +58,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -483,6 +488,346 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>In-vehicle</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>At-stop</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Extra</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Tardiness</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>FTNC</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>12.14893524930748</v>
+      </c>
+      <c r="C2" t="n">
+        <v>184.5303067413828</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>196.6792419906901</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>In-vehicle</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>At-stop</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Extra</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Tardiness</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>FTNC</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>14.7297870498615</v>
+      </c>
+      <c r="C2" t="n">
+        <v>189.4586169906902</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>75.18848069396029</v>
+      </c>
+      <c r="F2" t="n">
+        <v>279.3768847345121</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>In-vehicle</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>At-stop</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Extra</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Tardiness</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>FTNC</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>11.96169494459834</v>
+      </c>
+      <c r="C2" t="n">
+        <v>184.5360338881972</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>196.4977288327954</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>In-vehicle</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>At-stop</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Extra</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Tardiness</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>FTNC</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>10.71282029085873</v>
+      </c>
+      <c r="C2" t="n">
+        <v>182.7747665751778</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>193.4875868660364</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>In-vehicle</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>At-stop</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Extra</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Tardiness</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>FTNC</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>14.72926765927978</v>
+      </c>
+      <c r="C2" t="n">
+        <v>187.0297942760089</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>8.28313049376839</v>
+      </c>
+      <c r="F2" t="n">
+        <v>210.0421924290569</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
find a issue to retrieve model solution, still need to debug
</commit_message>
<xml_diff>
--- a/Results_ZC/results_Demand_5.xlsx
+++ b/Results_ZC/results_Demand_5.xlsx
@@ -1,18 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="FTNC_Demand5" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="FTNC_Demand51" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="FTNC_Demand52" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="FTNC_Demand53" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet name="FTNC_Demand54" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet name="FTNC_Demand55" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FTNC_Demand5" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FTNC_Demand51" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FTNC_Demand52" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FTNC_Demand53" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FTNC_Demand54" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FTNC_Demand55" sheetId="6" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -58,18 +58,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -472,23 +472,23 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>7.574835526315791</v>
+        <v>15.10426765927978</v>
       </c>
       <c r="C2" t="n">
-        <v>178.0098550639436</v>
+        <v>189.2671626970616</v>
       </c>
       <c r="D2" t="n">
         <v>0</v>
       </c>
       <c r="E2" t="n">
-        <v>2.229923522744834</v>
+        <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>187.8146141130041</v>
+        <v>204.371430356341</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -556,7 +556,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -624,7 +624,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -692,7 +692,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -760,7 +760,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
 
@@ -828,6 +828,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Analysis debug finished, average_analysis need to be debugged from line 920
</commit_message>
<xml_diff>
--- a/Results_ZC/results_Demand_5.xlsx
+++ b/Results_ZC/results_Demand_5.xlsx
@@ -1,18 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FTNC_Demand5" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FTNC_Demand51" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FTNC_Demand52" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FTNC_Demand53" sheetId="4" state="visible" r:id="rId4"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FTNC_Demand54" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="FTNC_Demand55" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="FTNC_Demand5" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="FTNC_Demand51" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="FTNC_Demand52" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="FTNC_Demand53" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="FTNC_Demand54" sheetId="5" state="visible" r:id="rId5"/>
+    <sheet name="FTNC_Demand55" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet name="FTNC_Demand56" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet name="FTNC_Demand57" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet name="FTNC_Demand58" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet name="FTNC_Demand59" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet name="FTNC_Demand510" sheetId="11" state="visible" r:id="rId11"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -58,18 +63,18 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="00000000"/>
@@ -488,7 +493,143 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>In-vehicle</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>At-stop</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Extra</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Tardiness</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>FTNC</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>8.646684556786706</v>
+      </c>
+      <c r="C2" t="n">
+        <v>178.8261308411057</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>4.956073777799302</v>
+      </c>
+      <c r="F2" t="n">
+        <v>192.4288891756918</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>In-vehicle</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>At-stop</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Extra</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Tardiness</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>FTNC</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>2285.421019712964</v>
+      </c>
+      <c r="C2" t="n">
+        <v>12672.64042375143</v>
+      </c>
+      <c r="D2" t="n">
+        <v>575.6307206712264</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>15533.6921641356</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -556,7 +697,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -624,7 +765,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -692,7 +833,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -760,7 +901,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
 
@@ -828,6 +969,210 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>In-vehicle</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>At-stop</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Extra</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Tardiness</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>FTNC</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>4.421875</v>
+      </c>
+      <c r="C2" t="n">
+        <v>221.8636545138889</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>226.2855295138889</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>In-vehicle</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>At-stop</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Extra</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Tardiness</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>FTNC</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>12.4249913434903</v>
+      </c>
+      <c r="C2" t="n">
+        <v>186.3187554948454</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0</v>
+      </c>
+      <c r="F2" t="n">
+        <v>198.7437468383357</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>In-vehicle</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>At-stop</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Extra</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Tardiness</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>FTNC</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>15.19801765927978</v>
+      </c>
+      <c r="C2" t="n">
+        <v>189.8765048023247</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>37.42165927533734</v>
+      </c>
+      <c r="F2" t="n">
+        <v>242.4961817369417</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>